<commit_message>
feat: update version to 1.1.4 and enhance template download functionality
</commit_message>
<xml_diff>
--- a/resources/templates/user-template.xlsx
+++ b/resources/templates/user-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZeMu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZEMU\8.OTHER_FILES\XAMPP\htdocs\INSA_psychometry_v2_desktop-app\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F9572E4-C93E-4E51-849E-C07C4397CE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F38A6F94-109F-4945-A830-F4FACB918198}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12828" yWindow="16404" windowWidth="17280" windowHeight="8880" xr2:uid="{DD01534E-C8F3-466C-9A4B-072B290A0397}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{DD01534E-C8F3-466C-9A4B-072B290A0397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Email</t>
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Zemu</t>
-  </si>
-  <si>
-    <t>zemu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,17 +413,9 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5716F1DF-CD0E-48E3-86B5-74A9FC3D056F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: enhance error handling and improve test status checks
</commit_message>
<xml_diff>
--- a/resources/templates/user-template.xlsx
+++ b/resources/templates/user-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZeMu\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ZEMU\8.OTHER_FILES\XAMPP\htdocs\INSA_psychometry_v2_desktop-app\resources\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F9572E4-C93E-4E51-849E-C07C4397CE0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35D19CC8-ED59-4F28-889A-32D2A65CD8F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12828" yWindow="16404" windowWidth="17280" windowHeight="8880" xr2:uid="{DD01534E-C8F3-466C-9A4B-072B290A0397}"/>
+    <workbookView xWindow="11016" yWindow="15264" windowWidth="17280" windowHeight="8880" xr2:uid="{DD01534E-C8F3-466C-9A4B-072B290A0397}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Email</t>
   </si>
   <si>
     <t>Name</t>
-  </si>
-  <si>
-    <t>Zemu</t>
-  </si>
-  <si>
-    <t>zemu@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +396,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -419,17 +413,9 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="B2" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{5716F1DF-CD0E-48E3-86B5-74A9FC3D056F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>